<commit_message>
Update division graph and XLS color chart
</commit_message>
<xml_diff>
--- a/R/Singapore_metadata.xlsx
+++ b/R/Singapore_metadata.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\daniel.vaulot@gmail.com\Metabarcoding\Singapore\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\daniel.vaulot@gmail.com\Metabarcoding\Singapore\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AC0D8B-AA36-4F47-B941-EE078C08AA99}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B774168-03CA-4393-94F7-8A8A245014AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11220" xr2:uid="{4D804F22-DFAA-47B5-8477-9C86D93AA77B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{4D804F22-DFAA-47B5-8477-9C86D93AA77B}"/>
   </bookViews>
   <sheets>
     <sheet name="samples" sheetId="1" r:id="rId1"/>
     <sheet name="stations" sheetId="3" r:id="rId2"/>
+    <sheet name="colors" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">samples!$A$1:$K$89</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="361">
   <si>
     <t>sample_id</t>
   </si>
@@ -863,13 +864,268 @@
   </si>
   <si>
     <t>longitude</t>
+  </si>
+  <si>
+    <t>division</t>
+  </si>
+  <si>
+    <t>Alphaproteobacteria</t>
+  </si>
+  <si>
+    <t>Bacteroidia</t>
+  </si>
+  <si>
+    <t>Gammaproteobacteria</t>
+  </si>
+  <si>
+    <t>Oxyphotobacteria</t>
+  </si>
+  <si>
+    <t>Nitrososphaeria</t>
+  </si>
+  <si>
+    <t>Thermoplasmata</t>
+  </si>
+  <si>
+    <t>Dinoflagellata</t>
+  </si>
+  <si>
+    <t>Acidimicrobiia</t>
+  </si>
+  <si>
+    <t>Ochrophyta</t>
+  </si>
+  <si>
+    <t>Chlorophyta</t>
+  </si>
+  <si>
+    <t>Marinimicrobia (SAR406 clade)</t>
+  </si>
+  <si>
+    <t>Actinobacteria</t>
+  </si>
+  <si>
+    <t>Bacteria</t>
+  </si>
+  <si>
+    <t>Planctomycetacia</t>
+  </si>
+  <si>
+    <t>Deltaproteobacteria</t>
+  </si>
+  <si>
+    <t>Ciliophora</t>
+  </si>
+  <si>
+    <t>Rhodothermia</t>
+  </si>
+  <si>
+    <t>Cryptophyta</t>
+  </si>
+  <si>
+    <t>OM190</t>
+  </si>
+  <si>
+    <t>Mollicutes</t>
+  </si>
+  <si>
+    <t>order_n_seq</t>
+  </si>
+  <si>
+    <t>Proteobacteria</t>
+  </si>
+  <si>
+    <t>Bacteroidetes</t>
+  </si>
+  <si>
+    <t>Cyanobacteria</t>
+  </si>
+  <si>
+    <t>Archaea</t>
+  </si>
+  <si>
+    <t>Thaumarchaeota</t>
+  </si>
+  <si>
+    <t>Euryarchaeota</t>
+  </si>
+  <si>
+    <t>Eukaryota</t>
+  </si>
+  <si>
+    <t>Alveolata</t>
+  </si>
+  <si>
+    <t>Stramenopiles</t>
+  </si>
+  <si>
+    <t>Archaeplastida</t>
+  </si>
+  <si>
+    <t>Planctomycetes</t>
+  </si>
+  <si>
+    <t>Hacrobia</t>
+  </si>
+  <si>
+    <t>Tenericutes</t>
+  </si>
+  <si>
+    <t>kingdom</t>
+  </si>
+  <si>
+    <t>supergroup</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>deeppink4</t>
+  </si>
+  <si>
+    <t>orchid4</t>
+  </si>
+  <si>
+    <t>plum3</t>
+  </si>
+  <si>
+    <t>dodgerblue4</t>
+  </si>
+  <si>
+    <t>steelblue</t>
+  </si>
+  <si>
+    <t>skyblue3</t>
+  </si>
+  <si>
+    <t>cadetblue</t>
+  </si>
+  <si>
+    <t>darkslategray3</t>
+  </si>
+  <si>
+    <t>springgreen4</t>
+  </si>
+  <si>
+    <t>mediumseagreen</t>
+  </si>
+  <si>
+    <t>darkseagreen3</t>
+  </si>
+  <si>
+    <t>goldenrod4</t>
+  </si>
+  <si>
+    <t>darkolivegreen3</t>
+  </si>
+  <si>
+    <t>lightgoldenrod</t>
+  </si>
+  <si>
+    <t>lightgoldenrod4</t>
+  </si>
+  <si>
+    <t>burlywood3</t>
+  </si>
+  <si>
+    <t>firebrick4</t>
+  </si>
+  <si>
+    <t>palevioletred</t>
+  </si>
+  <si>
+    <t>maroon</t>
+  </si>
+  <si>
+    <t>color_name</t>
+  </si>
+  <si>
+    <t>#771155</t>
+  </si>
+  <si>
+    <t>#AA4488</t>
+  </si>
+  <si>
+    <t>#CC99BB</t>
+  </si>
+  <si>
+    <t>#114477</t>
+  </si>
+  <si>
+    <t>#4477AA</t>
+  </si>
+  <si>
+    <t>#77AADD</t>
+  </si>
+  <si>
+    <t>#117777</t>
+  </si>
+  <si>
+    <t>#44AAAA</t>
+  </si>
+  <si>
+    <t>#77CCCC</t>
+  </si>
+  <si>
+    <t>#117744</t>
+  </si>
+  <si>
+    <t>#44AA77</t>
+  </si>
+  <si>
+    <t>#88CCAA</t>
+  </si>
+  <si>
+    <t>#777711</t>
+  </si>
+  <si>
+    <t>#AAAA44</t>
+  </si>
+  <si>
+    <t>#DDDD77</t>
+  </si>
+  <si>
+    <t>#774411</t>
+  </si>
+  <si>
+    <t>#AA7744</t>
+  </si>
+  <si>
+    <t>#DDAA77</t>
+  </si>
+  <si>
+    <t>#771122</t>
+  </si>
+  <si>
+    <t>#DD7788</t>
+  </si>
+  <si>
+    <t>#999099</t>
+  </si>
+  <si>
+    <t>#AA4455</t>
+  </si>
+  <si>
+    <t>saddlebrown</t>
+  </si>
+  <si>
+    <t>deepskyblue4</t>
+  </si>
+  <si>
+    <t>color_hex</t>
+  </si>
+  <si>
+    <t>gray90</t>
+  </si>
+  <si>
+    <t>Marinimicrobia (SAR406 clade)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -883,8 +1139,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -897,11 +1166,43 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4F8F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFD6DADC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD6DADC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFD6DADC"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -910,13 +1211,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1233,7 +1550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DD33BE-8376-466B-AC6A-1AAF9615F942}">
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
@@ -3521,4 +3838,486 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C19BF42-C5FA-4D9E-BC75-59DDE08983C7}">
+  <dimension ref="A1:AA25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="22.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E1" t="s">
+        <v>358</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+    </row>
+    <row r="2" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>14</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>15</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>17</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>19</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>20</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>7</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>9</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>10</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <v>18</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="E22" t="s">
+        <v>354</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:AA21">
+    <sortCondition ref="A17:A21"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update for revised version
</commit_message>
<xml_diff>
--- a/R/Singapore_metadata.xlsx
+++ b/R/Singapore_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\daniel.vaulot@gmail.com\Metabarcoding\Singapore\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B774168-03CA-4393-94F7-8A8A245014AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F9F83F-423D-4F8C-A269-306ACC996EA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{4D804F22-DFAA-47B5-8477-9C86D93AA77B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="425">
   <si>
     <t>sample_id</t>
   </si>
@@ -1119,6 +1119,198 @@
   </si>
   <si>
     <t>Marinimicrobia (SAR406 clade)</t>
+  </si>
+  <si>
+    <t>Flavobacteriales</t>
+  </si>
+  <si>
+    <t>Rhodobacterales</t>
+  </si>
+  <si>
+    <t>Synechococcales</t>
+  </si>
+  <si>
+    <t>Nitrosopumilales</t>
+  </si>
+  <si>
+    <t>SAR11 clade</t>
+  </si>
+  <si>
+    <t>Marine Group II</t>
+  </si>
+  <si>
+    <t>Cellvibrionales</t>
+  </si>
+  <si>
+    <t>Dinophyceae</t>
+  </si>
+  <si>
+    <t>SAR86 clade</t>
+  </si>
+  <si>
+    <t>Actinomarinales</t>
+  </si>
+  <si>
+    <t>Betaproteobacteriales</t>
+  </si>
+  <si>
+    <t>Oceanospirillales</t>
+  </si>
+  <si>
+    <t>Bacillariophyta</t>
+  </si>
+  <si>
+    <t>Microtrichales</t>
+  </si>
+  <si>
+    <t>Cytophagales</t>
+  </si>
+  <si>
+    <t>Chitinophagales</t>
+  </si>
+  <si>
+    <t>Syndiniales</t>
+  </si>
+  <si>
+    <t>Mamiellophyceae</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>Marine Group II</t>
+  </si>
+  <si>
+    <t>SAR11 clade</t>
+  </si>
+  <si>
+    <t>SAR86 clade</t>
+  </si>
+  <si>
+    <t>Rhodobacteraceae</t>
+  </si>
+  <si>
+    <t>Flavobacteriaceae</t>
+  </si>
+  <si>
+    <t>Cyanobiaceae</t>
+  </si>
+  <si>
+    <t>Nitrosopumilaceae</t>
+  </si>
+  <si>
+    <t>Halieaceae</t>
+  </si>
+  <si>
+    <t>Gymnodiniales</t>
+  </si>
+  <si>
+    <t>Actinomarinaceae</t>
+  </si>
+  <si>
+    <t>Cryomorphaceae</t>
+  </si>
+  <si>
+    <t>Crocinitomicaceae</t>
+  </si>
+  <si>
+    <t>Bacillariophyta_X</t>
+  </si>
+  <si>
+    <t>Nitrincolaceae</t>
+  </si>
+  <si>
+    <t>Burkholderiaceae</t>
+  </si>
+  <si>
+    <t>Cyclobacteriaceae</t>
+  </si>
+  <si>
+    <t>Ilumatobacteraceae</t>
+  </si>
+  <si>
+    <t>Clade I</t>
+  </si>
+  <si>
+    <t>NS9 marine group</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>color_name_old</t>
+  </si>
+  <si>
+    <t>Archeae</t>
+  </si>
+  <si>
+    <t>Bact</t>
+  </si>
+  <si>
+    <t>Euks</t>
+  </si>
+  <si>
+    <t>salmon1</t>
+  </si>
+  <si>
+    <t>firebrick2</t>
+  </si>
+  <si>
+    <t>lightsteelblue2</t>
+  </si>
+  <si>
+    <t>lightskyblue2</t>
+  </si>
+  <si>
+    <t>steelblue3</t>
+  </si>
+  <si>
+    <t>dodgerblue3</t>
+  </si>
+  <si>
+    <t>lightsteelblue</t>
+  </si>
+  <si>
+    <t>lightsteelblue3</t>
+  </si>
+  <si>
+    <t>mediumpurple3</t>
+  </si>
+  <si>
+    <t>mediumpurple4</t>
+  </si>
+  <si>
+    <t>purple4</t>
+  </si>
+  <si>
+    <t>honeydew</t>
+  </si>
+  <si>
+    <t>honeydew1</t>
+  </si>
+  <si>
+    <t>darkseagreen2</t>
+  </si>
+  <si>
+    <t>palegreen3</t>
+  </si>
+  <si>
+    <t>seagreen</t>
+  </si>
+  <si>
+    <t>seagreen4</t>
+  </si>
+  <si>
+    <t>ghostwhite</t>
+  </si>
+  <si>
+    <t>azure2</t>
+  </si>
+  <si>
+    <t>midnightblue</t>
+  </si>
+  <si>
+    <t>gray50</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1234,6 +1426,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3842,15 +4035,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C19BF42-C5FA-4D9E-BC75-59DDE08983C7}">
-  <dimension ref="A1:AA25"/>
+  <dimension ref="A1:AA59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="I30" sqref="I30:I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="4" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.375" customWidth="1"/>
+    <col min="14" max="15" width="13.5" customWidth="1"/>
+    <col min="21" max="21" width="14.125" customWidth="1"/>
+    <col min="22" max="22" width="23.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3873,23 +4072,52 @@
         <v>333</v>
       </c>
       <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="H1" t="s">
+        <v>297</v>
+      </c>
+      <c r="I1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J1" t="s">
+        <v>312</v>
+      </c>
+      <c r="K1" t="s">
+        <v>276</v>
+      </c>
+      <c r="L1" t="s">
+        <v>379</v>
+      </c>
+      <c r="M1" t="s">
+        <v>358</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>400</v>
+      </c>
       <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
+      <c r="R1" t="s">
+        <v>311</v>
+      </c>
+      <c r="S1" t="s">
+        <v>312</v>
+      </c>
+      <c r="T1" t="s">
+        <v>276</v>
+      </c>
+      <c r="U1" t="s">
+        <v>379</v>
+      </c>
+      <c r="V1" t="s">
+        <v>399</v>
+      </c>
+      <c r="W1" t="s">
+        <v>358</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>333</v>
+      </c>
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
@@ -3913,6 +4141,54 @@
       <c r="F2" s="4" t="s">
         <v>315</v>
       </c>
+      <c r="H2" s="6">
+        <v>4</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="N2" t="s">
+        <v>404</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>4</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="3" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
@@ -3933,6 +4209,54 @@
       <c r="F3" s="4" t="s">
         <v>316</v>
       </c>
+      <c r="H3" s="6">
+        <v>6</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="N3" t="s">
+        <v>405</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>6</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="4" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
@@ -3953,6 +4277,54 @@
       <c r="F4" s="4" t="s">
         <v>325</v>
       </c>
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="N4" t="s">
+        <v>421</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>1</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="5" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
@@ -3973,6 +4345,54 @@
       <c r="F5" s="4" t="s">
         <v>357</v>
       </c>
+      <c r="H5" s="6">
+        <v>2</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="N5" t="s">
+        <v>422</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>2</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="6" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
@@ -3993,6 +4413,54 @@
       <c r="F6" s="4" t="s">
         <v>328</v>
       </c>
+      <c r="H6" s="6">
+        <v>3</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="N6" t="s">
+        <v>410</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>3</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="7" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
@@ -4013,6 +4481,54 @@
       <c r="F7" s="4" t="s">
         <v>327</v>
       </c>
+      <c r="H7" s="6">
+        <v>5</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="N7" t="s">
+        <v>406</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>5</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="W7" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="8" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
@@ -4033,6 +4549,54 @@
       <c r="F8" s="4" t="s">
         <v>317</v>
       </c>
+      <c r="H8" s="6">
+        <v>7</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="N8" t="s">
+        <v>411</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>7</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="W8" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="X8" s="4" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="9" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
@@ -4053,6 +4617,54 @@
       <c r="F9" s="4" t="s">
         <v>329</v>
       </c>
+      <c r="H9" s="6">
+        <v>9</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="N9" t="s">
+        <v>407</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>8</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="W9" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="X9" s="4" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="10" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
@@ -4073,6 +4685,54 @@
       <c r="F10" s="4" t="s">
         <v>318</v>
       </c>
+      <c r="H10" s="6">
+        <v>10</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="N10" t="s">
+        <v>319</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>10</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="W10" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="X10" s="4" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="11" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
@@ -4093,6 +4753,54 @@
       <c r="F11" s="4" t="s">
         <v>319</v>
       </c>
+      <c r="H11" s="6">
+        <v>11</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="N11" t="s">
+        <v>408</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>11</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="W11" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="X11" s="4" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="12" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
@@ -4113,6 +4821,54 @@
       <c r="F12" s="4" t="s">
         <v>331</v>
       </c>
+      <c r="H12" s="6">
+        <v>12</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="N12" t="s">
+        <v>409</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>12</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="V12" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="W12" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="X12" s="4" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="13" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
@@ -4133,6 +4889,54 @@
       <c r="F13" s="4" t="s">
         <v>314</v>
       </c>
+      <c r="H13" s="6">
+        <v>14</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="N13" t="s">
+        <v>317</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>14</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="U13" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="V13" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="W13" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="X13" s="4" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="14" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
@@ -4153,6 +4957,54 @@
       <c r="F14" s="4" t="s">
         <v>320</v>
       </c>
+      <c r="H14" s="6">
+        <v>15</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="N14" t="s">
+        <v>412</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>15</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="U14" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="W14" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="X14" s="4" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="15" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
@@ -4173,6 +5025,54 @@
       <c r="F15" s="4" t="s">
         <v>330</v>
       </c>
+      <c r="H15" s="6">
+        <v>16</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="N15" t="s">
+        <v>413</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>16</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="U15" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="V15" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="W15" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="X15" s="4" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="16" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
@@ -4193,8 +5093,56 @@
       <c r="F16" s="4" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="6">
+        <v>17</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="N16" t="s">
+        <v>414</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>17</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="U16" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="V16" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="W16" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="X16" s="4" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>7</v>
       </c>
@@ -4213,8 +5161,56 @@
       <c r="F17" s="4" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="6">
+        <v>18</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="N17" t="s">
+        <v>423</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>18</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="S17" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="U17" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="V17" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="W17" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="X17" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>9</v>
       </c>
@@ -4233,8 +5229,56 @@
       <c r="F18" s="4" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="6">
+        <v>8</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="N18" t="s">
+        <v>417</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>19</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="T18" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="U18" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="V18" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="W18" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="X18" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>10</v>
       </c>
@@ -4253,8 +5297,56 @@
       <c r="F19" s="4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H19" s="6">
+        <v>13</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="N19" t="s">
+        <v>418</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>20</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="T19" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="U19" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="V19" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="W19" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="X19" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>16</v>
       </c>
@@ -4273,8 +5365,56 @@
       <c r="F20" s="4" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H20" s="6">
+        <v>19</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="N20" t="s">
+        <v>419</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="Q20" s="6">
+        <v>9</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="T20" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="U20" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="V20" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="W20" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="X20" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>18</v>
       </c>
@@ -4293,8 +5433,56 @@
       <c r="F21" s="4" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="6">
+        <v>20</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="N21" t="s">
+        <v>420</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="Q21" s="6">
+        <v>13</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="T21" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="U21" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="V21" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="W21" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="X21" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="7" t="s">
         <v>313</v>
       </c>
@@ -4304,20 +5492,98 @@
       <c r="F22" s="4" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L22" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="M22" t="s">
+        <v>354</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="V22" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="W22" t="s">
+        <v>354</v>
+      </c>
+      <c r="X22" s="4" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M24" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="N24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E25" s="5" t="s">
         <v>342</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>321</v>
       </c>
+      <c r="M25" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="N25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M26" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="N26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I53" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="54" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I54" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="55" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I55" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="56" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I56" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="57" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I57" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="58" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I58" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="59" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I59" t="s">
+        <v>420</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:AA21">
-    <sortCondition ref="A17:A21"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A13:AA22">
+    <sortCondition ref="A13:A22"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>